<commit_message>
landing page html & css (_layout) all devices + initial _collection css improvement. also added some IOS specific media queries cause i think we'll need those
</commit_message>
<xml_diff>
--- a/documents/lb_backlog.xlsx
+++ b/documents/lb_backlog.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="293">
   <si>
     <t>accepts payment methods: cc, paypal, btc, ideal, direct bank transfer ...
 Make your payment directly into our bank account. Please use your Order ID as the payment reference. Your order won’t be shipped until the funds have cleared in our account.
@@ -1043,7 +1043,19 @@
     <t>move object info in store page to center collumn?</t>
   </si>
   <si>
-    <t>discuss with girls</t>
+    <t>implement method to link/share product specific page in collection</t>
+  </si>
+  <si>
+    <t>discussed with girls, agreed, done</t>
+  </si>
+  <si>
+    <t>resize landing page images (object,image,download)</t>
+  </si>
+  <si>
+    <t>way too big right now</t>
+  </si>
+  <si>
+    <t>style css for IOS device</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1067,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.00_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1105,6 +1117,12 @@
       <sz val="10"/>
       <color rgb="FF252525"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1189,12 +1207,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1253,7 +1272,8 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2858,8 +2878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3483,28 +3503,76 @@
         <v>272</v>
       </c>
       <c r="E38" t="s">
-        <v>274</v>
+        <v>58</v>
       </c>
       <c r="F38" t="s">
         <v>268</v>
       </c>
       <c r="G38" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39">
         <v>28</v>
       </c>
+      <c r="B39" t="s">
+        <v>288</v>
+      </c>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" t="s">
+        <v>272</v>
+      </c>
+      <c r="E39" t="s">
+        <v>274</v>
+      </c>
+      <c r="F39" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40">
         <v>29</v>
       </c>
+      <c r="B40" t="s">
+        <v>290</v>
+      </c>
+      <c r="C40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" t="s">
+        <v>272</v>
+      </c>
+      <c r="E40" t="s">
+        <v>274</v>
+      </c>
+      <c r="F40" t="s">
+        <v>268</v>
+      </c>
+      <c r="G40" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41">
         <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>292</v>
+      </c>
+      <c r="C41" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" t="s">
+        <v>272</v>
+      </c>
+      <c r="E41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -3521,11 +3589,12 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D44">
       <formula1>$K$1:$K$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:E39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:E57">
       <formula1>$L$1:$L$13</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
content-pages 1st draft added, devices.css (iOS) added, tweaks and updates on most css files, landing page changes
</commit_message>
<xml_diff>
--- a/documents/lb_backlog.xlsx
+++ b/documents/lb_backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="requirements" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="status" sheetId="6" r:id="rId6"/>
     <sheet name="backlog" sheetId="7" r:id="rId7"/>
     <sheet name="models" sheetId="8" r:id="rId8"/>
+    <sheet name="optimisation" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="297">
   <si>
     <t>accepts payment methods: cc, paypal, btc, ideal, direct bank transfer ...
 Make your payment directly into our bank account. Please use your Order ID as the payment reference. Your order won’t be shipped until the funds have cleared in our account.
@@ -1056,6 +1057,18 @@
   </si>
   <si>
     <t>style css for IOS device</t>
+  </si>
+  <si>
+    <t>get more testimonials</t>
+  </si>
+  <si>
+    <t>show views/status/sells of products</t>
+  </si>
+  <si>
+    <t>better impressions of what people get when they buy</t>
+  </si>
+  <si>
+    <t>implement shopping cart</t>
   </si>
 </sst>
 </file>
@@ -1063,9 +1076,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="6" formatCode="&quot;€&quot;#,##0_);[Red]\(&quot;€&quot;#,##0\)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.00_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;#,##0_);[Red]\(&quot;€&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0.00_-"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1125,12 +1138,30 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -1215,7 +1246,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1248,29 +1279,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2076,14 +2110,14 @@
   <sheetData>
     <row r="7" spans="2:6">
       <c r="B7" s="8"/>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31" t="s">
+      <c r="D7" s="32"/>
+      <c r="E7" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="31"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="9" t="s">
@@ -2820,7 +2854,7 @@
   <dimension ref="B5:B11"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2878,8 +2912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2964,7 +2998,7 @@
       <c r="D12" t="s">
         <v>146</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F12" t="s">
@@ -2987,7 +3021,7 @@
       <c r="D13" t="s">
         <v>146</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F13" t="s">
@@ -3010,7 +3044,7 @@
       <c r="D14" t="s">
         <v>146</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="34" t="s">
         <v>65</v>
       </c>
       <c r="F14" t="s">
@@ -3030,7 +3064,7 @@
       <c r="D15" t="s">
         <v>272</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="34" t="s">
         <v>65</v>
       </c>
       <c r="F15" t="s">
@@ -3050,7 +3084,7 @@
       <c r="D16" t="s">
         <v>272</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="34" t="s">
         <v>65</v>
       </c>
       <c r="F16" t="s">
@@ -3070,7 +3104,7 @@
       <c r="D17" t="s">
         <v>272</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="34" t="s">
         <v>65</v>
       </c>
       <c r="F17" t="s">
@@ -3090,7 +3124,7 @@
       <c r="D18" t="s">
         <v>272</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="34" t="s">
         <v>65</v>
       </c>
       <c r="F18" t="s">
@@ -3110,7 +3144,7 @@
       <c r="D19" t="s">
         <v>146</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="33" t="s">
         <v>59</v>
       </c>
       <c r="F19" t="s">
@@ -3130,7 +3164,7 @@
       <c r="D20" t="s">
         <v>272</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F20" t="s">
@@ -3150,7 +3184,7 @@
       <c r="D21" t="s">
         <v>146</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="34" t="s">
         <v>65</v>
       </c>
       <c r="F21" t="s">
@@ -3170,7 +3204,7 @@
       <c r="D22" t="s">
         <v>272</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F22" t="s">
@@ -3193,7 +3227,7 @@
       <c r="D23" t="s">
         <v>273</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="35" t="s">
         <v>274</v>
       </c>
       <c r="F23" t="s">
@@ -3213,7 +3247,7 @@
       <c r="D24" t="s">
         <v>272</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F24" t="s">
@@ -3233,7 +3267,7 @@
       <c r="D25" t="s">
         <v>146</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="34" t="s">
         <v>65</v>
       </c>
       <c r="F25" t="s">
@@ -3253,7 +3287,7 @@
       <c r="D26" t="s">
         <v>146</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="34" t="s">
         <v>65</v>
       </c>
       <c r="F26" t="s">
@@ -3276,7 +3310,7 @@
       <c r="D27" t="s">
         <v>146</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F27" t="s">
@@ -3299,7 +3333,7 @@
       <c r="D28" t="s">
         <v>146</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F28" t="s">
@@ -3319,7 +3353,7 @@
       <c r="D29" t="s">
         <v>273</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="35" t="s">
         <v>274</v>
       </c>
       <c r="F29" t="s">
@@ -3339,7 +3373,7 @@
       <c r="D30" t="s">
         <v>146</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="34" t="s">
         <v>65</v>
       </c>
       <c r="F30" t="s">
@@ -3359,7 +3393,7 @@
       <c r="D31" t="s">
         <v>272</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="35" t="s">
         <v>274</v>
       </c>
       <c r="F31" t="s">
@@ -3379,7 +3413,7 @@
       <c r="D32" t="s">
         <v>272</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="34" t="s">
         <v>65</v>
       </c>
       <c r="F32" t="s">
@@ -3399,7 +3433,7 @@
       <c r="D33" t="s">
         <v>273</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="35" t="s">
         <v>274</v>
       </c>
       <c r="F33" t="s">
@@ -3419,7 +3453,7 @@
       <c r="D34" t="s">
         <v>273</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="35" t="s">
         <v>274</v>
       </c>
       <c r="F34" t="s">
@@ -3439,13 +3473,13 @@
       <c r="D35" t="s">
         <v>273</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="35" t="s">
         <v>274</v>
       </c>
       <c r="F35" t="s">
         <v>270</v>
       </c>
-      <c r="G35" s="32" t="s">
+      <c r="G35" s="31" t="s">
         <v>284</v>
       </c>
     </row>
@@ -3462,7 +3496,7 @@
       <c r="D36" t="s">
         <v>272</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="35" t="s">
         <v>274</v>
       </c>
       <c r="F36" t="s">
@@ -3482,7 +3516,7 @@
       <c r="D37" t="s">
         <v>273</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="35" t="s">
         <v>274</v>
       </c>
       <c r="F37" t="s">
@@ -3502,7 +3536,7 @@
       <c r="D38" t="s">
         <v>272</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F38" t="s">
@@ -3525,7 +3559,7 @@
       <c r="D39" t="s">
         <v>272</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="35" t="s">
         <v>274</v>
       </c>
       <c r="F39" t="s">
@@ -3545,7 +3579,7 @@
       <c r="D40" t="s">
         <v>272</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="35" t="s">
         <v>274</v>
       </c>
       <c r="F40" t="s">
@@ -3568,7 +3602,7 @@
       <c r="D41" t="s">
         <v>272</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="34" t="s">
         <v>65</v>
       </c>
       <c r="F41" t="s">
@@ -3819,4 +3853,47 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="66.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>